<commit_message>
Made more edits to Game Div
</commit_message>
<xml_diff>
--- a/assets/Logic Square References.xlsx
+++ b/assets/Logic Square References.xlsx
@@ -20,9 +20,249 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="82">
+  <si>
+    <t xml:space="preserve">`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`92</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`24</t>
+  </si>
   <si>
     <t xml:space="preserve">this</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`15</t>
   </si>
   <si>
     <t xml:space="preserve">Make an array for all elements starting with top Div left to right then left Div left to right top to bottom</t>
@@ -40,6 +280,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -57,7 +298,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -68,6 +309,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF87D1D1"/>
         <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF200"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -112,7 +359,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -122,6 +369,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -141,7 +396,7 @@
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFFF200"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
@@ -202,29 +457,77 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="G5:BP64"/>
+  <dimension ref="G5:CE68"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AE70" activeCellId="0" sqref="AE70"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AE32" activeCellId="0" sqref="AE32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="17.3" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="2.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="3.11"/>
   </cols>
   <sheetData>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="Q5" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="R5" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="S5" s="0" t="n">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="U5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="V5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="W5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="X5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K6" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="L6" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="O6" s="0" t="n">
         <v>3</v>
       </c>
@@ -246,11 +549,20 @@
       <c r="U6" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="V6" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="W6" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="X6" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="Y6" s="0" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K7" s="0" t="n">
         <v>3</v>
       </c>
@@ -297,7 +609,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K8" s="0" t="n">
         <v>4</v>
       </c>
@@ -344,7 +656,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G9" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="H9" s="0" t="n">
         <v>4</v>
       </c>
@@ -354,21 +669,43 @@
       <c r="J9" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
+      <c r="K9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M9" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="N9" s="1" t="n">
+        <v>3</v>
+      </c>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
+      <c r="Q9" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="R9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="S9" s="1" t="n">
+        <v>8</v>
+      </c>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
-      <c r="V9" s="1"/>
-      <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
-      <c r="Y9" s="1"/>
+      <c r="V9" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="W9" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="X9" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="Y9" s="1" t="n">
+        <v>14</v>
+      </c>
       <c r="AC9" s="2"/>
       <c r="AD9" s="2"/>
       <c r="AE9" s="2"/>
@@ -399,26 +736,80 @@
       <c r="BG9" s="2"/>
       <c r="BH9" s="2"/>
       <c r="BI9" s="2"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BQ9" s="3"/>
+      <c r="BR9" s="3"/>
+      <c r="BS9" s="3"/>
+      <c r="BT9" s="3"/>
+      <c r="BU9" s="3"/>
+      <c r="BV9" s="3"/>
+      <c r="BW9" s="3"/>
+      <c r="BX9" s="3"/>
+      <c r="BY9" s="3"/>
+      <c r="BZ9" s="3"/>
+      <c r="CA9" s="3"/>
+      <c r="CB9" s="3"/>
+      <c r="CC9" s="3"/>
+      <c r="CD9" s="3"/>
+      <c r="CE9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G10" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="J10" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
+      <c r="K10" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="L10" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="M10" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="N10" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="O10" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="P10" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q10" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="R10" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="S10" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="T10" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="U10" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="V10" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="W10" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="X10" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="Y10" s="1" t="n">
+        <v>29</v>
+      </c>
       <c r="AC10" s="2"/>
       <c r="AD10" s="2"/>
       <c r="AE10" s="2"/>
@@ -449,26 +840,80 @@
       <c r="BG10" s="1"/>
       <c r="BH10" s="1"/>
       <c r="BI10" s="1"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BQ10" s="3"/>
+      <c r="BR10" s="3"/>
+      <c r="BS10" s="3"/>
+      <c r="BT10" s="3"/>
+      <c r="BU10" s="3"/>
+      <c r="BV10" s="3"/>
+      <c r="BW10" s="1"/>
+      <c r="BX10" s="1"/>
+      <c r="BY10" s="1"/>
+      <c r="BZ10" s="3"/>
+      <c r="CA10" s="3"/>
+      <c r="CB10" s="3"/>
+      <c r="CC10" s="3"/>
+      <c r="CD10" s="3"/>
+      <c r="CE10" s="3"/>
+    </row>
+    <row r="11" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G11" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="J11" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
-      <c r="W11" s="1"/>
-      <c r="X11" s="1"/>
-      <c r="Y11" s="1"/>
+      <c r="K11" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="L11" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="M11" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="N11" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="O11" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="P11" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q11" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="R11" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="S11" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="T11" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="U11" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="V11" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="W11" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="X11" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="Y11" s="1" t="n">
+        <v>44</v>
+      </c>
       <c r="AC11" s="2"/>
       <c r="AD11" s="2"/>
       <c r="AE11" s="1"/>
@@ -499,8 +944,26 @@
       <c r="BG11" s="2"/>
       <c r="BH11" s="2"/>
       <c r="BI11" s="1"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BQ11" s="3"/>
+      <c r="BR11" s="3"/>
+      <c r="BS11" s="3"/>
+      <c r="BT11" s="3"/>
+      <c r="BU11" s="1"/>
+      <c r="BV11" s="1"/>
+      <c r="BW11" s="1"/>
+      <c r="BX11" s="1"/>
+      <c r="BY11" s="1"/>
+      <c r="BZ11" s="1"/>
+      <c r="CA11" s="3"/>
+      <c r="CB11" s="3"/>
+      <c r="CC11" s="3"/>
+      <c r="CD11" s="3"/>
+      <c r="CE11" s="3"/>
+    </row>
+    <row r="12" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G12" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="H12" s="0" t="n">
         <v>1</v>
       </c>
@@ -510,21 +973,43 @@
       <c r="J12" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K12" s="1"/>
+      <c r="K12" s="1" t="n">
+        <v>45</v>
+      </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
-      <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
+      <c r="N12" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="O12" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="P12" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q12" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="R12" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="S12" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="T12" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="U12" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="V12" s="1" t="n">
+        <v>56</v>
+      </c>
       <c r="W12" s="2"/>
       <c r="X12" s="2"/>
-      <c r="Y12" s="1"/>
+      <c r="Y12" s="1" t="n">
+        <v>59</v>
+      </c>
       <c r="AC12" s="2"/>
       <c r="AD12" s="1"/>
       <c r="AE12" s="2"/>
@@ -555,8 +1040,29 @@
       <c r="BG12" s="2"/>
       <c r="BH12" s="1"/>
       <c r="BI12" s="2"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BQ12" s="3"/>
+      <c r="BR12" s="3"/>
+      <c r="BS12" s="3"/>
+      <c r="BT12" s="1"/>
+      <c r="BU12" s="1"/>
+      <c r="BV12" s="1"/>
+      <c r="BW12" s="3"/>
+      <c r="BX12" s="3"/>
+      <c r="BY12" s="3"/>
+      <c r="BZ12" s="1"/>
+      <c r="CA12" s="1"/>
+      <c r="CB12" s="3"/>
+      <c r="CC12" s="3"/>
+      <c r="CD12" s="3"/>
+      <c r="CE12" s="3"/>
+    </row>
+    <row r="13" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G13" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="I13" s="0" t="n">
         <v>1</v>
       </c>
@@ -564,7 +1070,9 @@
         <v>1</v>
       </c>
       <c r="K13" s="2"/>
-      <c r="L13" s="1"/>
+      <c r="L13" s="1" t="n">
+        <v>61</v>
+      </c>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -576,7 +1084,9 @@
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
-      <c r="X13" s="1"/>
+      <c r="X13" s="1" t="n">
+        <v>73</v>
+      </c>
       <c r="Y13" s="2"/>
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
@@ -608,8 +1118,29 @@
       <c r="BG13" s="1"/>
       <c r="BH13" s="2"/>
       <c r="BI13" s="2"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BQ13" s="3"/>
+      <c r="BR13" s="3"/>
+      <c r="BS13" s="3"/>
+      <c r="BT13" s="1"/>
+      <c r="BU13" s="1"/>
+      <c r="BV13" s="3"/>
+      <c r="BW13" s="3"/>
+      <c r="BX13" s="3"/>
+      <c r="BY13" s="3"/>
+      <c r="BZ13" s="3"/>
+      <c r="CA13" s="1"/>
+      <c r="CB13" s="1"/>
+      <c r="CC13" s="3"/>
+      <c r="CD13" s="3"/>
+      <c r="CE13" s="3"/>
+    </row>
+    <row r="14" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G14" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="I14" s="0" t="n">
         <v>2</v>
       </c>
@@ -617,8 +1148,12 @@
         <v>2</v>
       </c>
       <c r="K14" s="2"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
+      <c r="L14" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="M14" s="1" t="n">
+        <v>77</v>
+      </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
@@ -628,8 +1163,12 @@
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
-      <c r="W14" s="1"/>
-      <c r="X14" s="1"/>
+      <c r="W14" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="X14" s="1" t="n">
+        <v>88</v>
+      </c>
       <c r="Y14" s="2"/>
       <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
@@ -661,8 +1200,23 @@
       <c r="BG14" s="2"/>
       <c r="BH14" s="2"/>
       <c r="BI14" s="2"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BQ14" s="3"/>
+      <c r="BR14" s="3"/>
+      <c r="BS14" s="3"/>
+      <c r="BT14" s="3"/>
+      <c r="BU14" s="3"/>
+      <c r="BV14" s="3"/>
+      <c r="BW14" s="3"/>
+      <c r="BX14" s="3"/>
+      <c r="BY14" s="3"/>
+      <c r="BZ14" s="3"/>
+      <c r="CA14" s="1"/>
+      <c r="CB14" s="1"/>
+      <c r="CC14" s="3"/>
+      <c r="CD14" s="3"/>
+      <c r="CE14" s="3"/>
+    </row>
+    <row r="15" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G15" s="0" t="n">
         <v>3</v>
       </c>
@@ -675,21 +1229,45 @@
       <c r="J15" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
+      <c r="K15" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="L15" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="M15" s="1" t="n">
+        <v>92</v>
+      </c>
       <c r="N15" s="2"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
+      <c r="O15" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="P15" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="Q15" s="1" t="n">
+        <v>96</v>
+      </c>
       <c r="R15" s="2"/>
-      <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
-      <c r="U15" s="1"/>
+      <c r="S15" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="T15" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="U15" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="V15" s="2"/>
-      <c r="W15" s="1"/>
-      <c r="X15" s="1"/>
-      <c r="Y15" s="1"/>
+      <c r="W15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="X15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y15" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="AC15" s="1"/>
       <c r="AD15" s="2"/>
       <c r="AE15" s="1"/>
@@ -720,8 +1298,23 @@
       <c r="BG15" s="1"/>
       <c r="BH15" s="1"/>
       <c r="BI15" s="2"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BQ15" s="3"/>
+      <c r="BR15" s="3"/>
+      <c r="BS15" s="3"/>
+      <c r="BT15" s="3"/>
+      <c r="BU15" s="3"/>
+      <c r="BV15" s="3"/>
+      <c r="BW15" s="3"/>
+      <c r="BX15" s="3"/>
+      <c r="BY15" s="3"/>
+      <c r="BZ15" s="3"/>
+      <c r="CA15" s="1"/>
+      <c r="CB15" s="1"/>
+      <c r="CC15" s="3"/>
+      <c r="CD15" s="3"/>
+      <c r="CE15" s="3"/>
+    </row>
+    <row r="16" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G16" s="0" t="n">
         <v>3</v>
       </c>
@@ -734,21 +1327,37 @@
       <c r="J16" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
+      <c r="K16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
-      <c r="P16" s="1"/>
+      <c r="P16" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
-      <c r="T16" s="1"/>
+      <c r="T16" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
-      <c r="W16" s="1"/>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
+      <c r="W16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y16" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="AC16" s="1"/>
       <c r="AD16" s="2"/>
       <c r="AE16" s="1"/>
@@ -779,17 +1388,44 @@
       <c r="BG16" s="2"/>
       <c r="BH16" s="1"/>
       <c r="BI16" s="2"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BQ16" s="3"/>
+      <c r="BR16" s="3"/>
+      <c r="BS16" s="3"/>
+      <c r="BT16" s="3"/>
+      <c r="BU16" s="3"/>
+      <c r="BV16" s="3"/>
+      <c r="BW16" s="1"/>
+      <c r="BX16" s="1"/>
+      <c r="BY16" s="1"/>
+      <c r="BZ16" s="1"/>
+      <c r="CA16" s="1"/>
+      <c r="CB16" s="3"/>
+      <c r="CC16" s="3"/>
+      <c r="CD16" s="3"/>
+      <c r="CE16" s="3"/>
+    </row>
+    <row r="17" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G17" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="I17" s="0" t="n">
         <v>3</v>
       </c>
       <c r="J17" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
+      <c r="K17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
@@ -799,9 +1435,15 @@
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
-      <c r="W17" s="1"/>
-      <c r="X17" s="1"/>
-      <c r="Y17" s="1"/>
+      <c r="W17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="X17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y17" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="AC17" s="1"/>
       <c r="AD17" s="2"/>
       <c r="AE17" s="2"/>
@@ -832,8 +1474,26 @@
       <c r="BG17" s="1"/>
       <c r="BH17" s="2"/>
       <c r="BI17" s="2"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BQ17" s="3"/>
+      <c r="BR17" s="3"/>
+      <c r="BS17" s="3"/>
+      <c r="BT17" s="3"/>
+      <c r="BU17" s="3"/>
+      <c r="BV17" s="1"/>
+      <c r="BW17" s="1"/>
+      <c r="BX17" s="1"/>
+      <c r="BY17" s="1"/>
+      <c r="BZ17" s="1"/>
+      <c r="CA17" s="1"/>
+      <c r="CB17" s="3"/>
+      <c r="CC17" s="3"/>
+      <c r="CD17" s="3"/>
+      <c r="CE17" s="3"/>
+    </row>
+    <row r="18" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G18" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="H18" s="0" t="n">
         <v>3</v>
       </c>
@@ -844,9 +1504,15 @@
         <v>3</v>
       </c>
       <c r="K18" s="2"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
+      <c r="L18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
@@ -854,9 +1520,15 @@
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
-      <c r="V18" s="1"/>
-      <c r="W18" s="1"/>
-      <c r="X18" s="1"/>
+      <c r="V18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="W18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="X18" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="Y18" s="2"/>
       <c r="AC18" s="1"/>
       <c r="AD18" s="2"/>
@@ -888,8 +1560,26 @@
       <c r="BG18" s="1"/>
       <c r="BH18" s="1"/>
       <c r="BI18" s="2"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BQ18" s="3"/>
+      <c r="BR18" s="3"/>
+      <c r="BS18" s="3"/>
+      <c r="BT18" s="3"/>
+      <c r="BU18" s="3"/>
+      <c r="BV18" s="1"/>
+      <c r="BW18" s="1"/>
+      <c r="BX18" s="3"/>
+      <c r="BY18" s="3"/>
+      <c r="BZ18" s="3"/>
+      <c r="CA18" s="3"/>
+      <c r="CB18" s="3"/>
+      <c r="CC18" s="3"/>
+      <c r="CD18" s="3"/>
+      <c r="CE18" s="3"/>
+    </row>
+    <row r="19" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G19" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="H19" s="0" t="n">
         <v>3</v>
       </c>
@@ -900,19 +1590,33 @@
         <v>3</v>
       </c>
       <c r="K19" s="2"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
+      <c r="L19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
-      <c r="R19" s="1"/>
+      <c r="R19" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
-      <c r="V19" s="1"/>
-      <c r="W19" s="1"/>
-      <c r="X19" s="1"/>
+      <c r="V19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="X19" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="Y19" s="2"/>
       <c r="AC19" s="1"/>
       <c r="AD19" s="1"/>
@@ -944,8 +1648,23 @@
       <c r="BG19" s="1"/>
       <c r="BH19" s="2"/>
       <c r="BI19" s="2"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BQ19" s="3"/>
+      <c r="BR19" s="3"/>
+      <c r="BS19" s="3"/>
+      <c r="BT19" s="3"/>
+      <c r="BU19" s="3"/>
+      <c r="BV19" s="1"/>
+      <c r="BW19" s="1"/>
+      <c r="BX19" s="3"/>
+      <c r="BY19" s="3"/>
+      <c r="BZ19" s="3"/>
+      <c r="CA19" s="3"/>
+      <c r="CB19" s="3"/>
+      <c r="CC19" s="3"/>
+      <c r="CD19" s="3"/>
+      <c r="CE19" s="3"/>
+    </row>
+    <row r="20" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G20" s="0" t="n">
         <v>4</v>
       </c>
@@ -958,21 +1677,41 @@
       <c r="J20" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
+      <c r="K20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
-      <c r="Q20" s="1"/>
+      <c r="Q20" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="R20" s="2"/>
-      <c r="S20" s="1"/>
+      <c r="S20" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
-      <c r="V20" s="1"/>
-      <c r="W20" s="1"/>
-      <c r="X20" s="1"/>
-      <c r="Y20" s="1"/>
+      <c r="V20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y20" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="AC20" s="2"/>
       <c r="AD20" s="1"/>
       <c r="AE20" s="2"/>
@@ -1003,29 +1742,70 @@
       <c r="BG20" s="2"/>
       <c r="BH20" s="2"/>
       <c r="BI20" s="2"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BQ20" s="3"/>
+      <c r="BR20" s="3"/>
+      <c r="BS20" s="3"/>
+      <c r="BT20" s="3"/>
+      <c r="BU20" s="3"/>
+      <c r="BV20" s="3"/>
+      <c r="BW20" s="3"/>
+      <c r="BX20" s="3"/>
+      <c r="BY20" s="3"/>
+      <c r="BZ20" s="3"/>
+      <c r="CA20" s="3"/>
+      <c r="CB20" s="3"/>
+      <c r="CC20" s="3"/>
+      <c r="CD20" s="3"/>
+      <c r="CE20" s="3"/>
+    </row>
+    <row r="21" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G21" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="I21" s="0" t="n">
         <v>5</v>
       </c>
       <c r="J21" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
+      <c r="K21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
-      <c r="U21" s="1"/>
-      <c r="V21" s="1"/>
-      <c r="W21" s="1"/>
-      <c r="X21" s="1"/>
-      <c r="Y21" s="1"/>
+      <c r="U21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y21" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="AC21" s="2"/>
       <c r="AD21" s="2"/>
       <c r="AE21" s="1"/>
@@ -1056,26 +1836,80 @@
       <c r="BG21" s="2"/>
       <c r="BH21" s="2"/>
       <c r="BI21" s="2"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BQ21" s="3"/>
+      <c r="BR21" s="3"/>
+      <c r="BS21" s="3"/>
+      <c r="BT21" s="3"/>
+      <c r="BU21" s="3"/>
+      <c r="BV21" s="1"/>
+      <c r="BW21" s="1"/>
+      <c r="BX21" s="3"/>
+      <c r="BY21" s="3"/>
+      <c r="BZ21" s="3"/>
+      <c r="CA21" s="3"/>
+      <c r="CB21" s="3"/>
+      <c r="CC21" s="3"/>
+      <c r="CD21" s="3"/>
+      <c r="CE21" s="3"/>
+    </row>
+    <row r="22" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G22" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="J22" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
-      <c r="T22" s="1"/>
-      <c r="U22" s="1"/>
-      <c r="V22" s="1"/>
-      <c r="W22" s="1"/>
-      <c r="X22" s="1"/>
-      <c r="Y22" s="1"/>
+      <c r="K22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="W22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="X22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y22" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="AC22" s="2"/>
       <c r="AD22" s="2"/>
       <c r="AE22" s="2"/>
@@ -1106,8 +1940,26 @@
       <c r="BG22" s="2"/>
       <c r="BH22" s="2"/>
       <c r="BI22" s="2"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BQ22" s="3"/>
+      <c r="BR22" s="3"/>
+      <c r="BS22" s="3"/>
+      <c r="BT22" s="3"/>
+      <c r="BU22" s="3"/>
+      <c r="BV22" s="1"/>
+      <c r="BW22" s="1"/>
+      <c r="BX22" s="3"/>
+      <c r="BY22" s="3"/>
+      <c r="BZ22" s="3"/>
+      <c r="CA22" s="3"/>
+      <c r="CB22" s="3"/>
+      <c r="CC22" s="3"/>
+      <c r="CD22" s="3"/>
+      <c r="CE22" s="3"/>
+    </row>
+    <row r="23" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G23" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="H23" s="0" t="n">
         <v>4</v>
       </c>
@@ -1117,21 +1969,43 @@
       <c r="J23" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
+      <c r="K23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
+      <c r="Q23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
-      <c r="V23" s="1"/>
-      <c r="W23" s="1"/>
-      <c r="X23" s="1"/>
-      <c r="Y23" s="1"/>
+      <c r="V23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="W23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="X23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y23" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="AC23" s="2"/>
       <c r="AD23" s="2"/>
       <c r="AE23" s="2"/>
@@ -1162,13 +2036,33 @@
       <c r="BG23" s="2"/>
       <c r="BH23" s="2"/>
       <c r="BI23" s="2"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BQ23" s="3"/>
+      <c r="BR23" s="3"/>
+      <c r="BS23" s="3"/>
+      <c r="BT23" s="3"/>
+      <c r="BU23" s="3"/>
+      <c r="BV23" s="3"/>
+      <c r="BW23" s="3"/>
+      <c r="BX23" s="3"/>
+      <c r="BY23" s="3"/>
+      <c r="BZ23" s="3"/>
+      <c r="CA23" s="3"/>
+      <c r="CB23" s="3"/>
+      <c r="CC23" s="3"/>
+      <c r="CD23" s="3"/>
+      <c r="CE23" s="3"/>
+    </row>
+    <row r="24" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="R24" s="0" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="V30" s="0" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O31" s="0" t="n">
         <v>1</v>
       </c>
@@ -1176,7 +2070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="L32" s="0" t="n">
         <v>5</v>
       </c>
@@ -1217,7 +2111,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="L33" s="0" t="n">
         <v>3</v>
       </c>
@@ -1258,7 +2152,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K34" s="0" t="n">
         <v>13</v>
       </c>
@@ -1305,17 +2199,25 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="I35" s="0" t="n">
         <v>4</v>
       </c>
       <c r="J35" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
+      <c r="K35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L35" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M35" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="N35" s="1" t="n">
+        <v>3</v>
+      </c>
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
@@ -1323,10 +2225,18 @@
       <c r="S35" s="2"/>
       <c r="T35" s="2"/>
       <c r="U35" s="2"/>
-      <c r="V35" s="1"/>
-      <c r="W35" s="1"/>
-      <c r="X35" s="1"/>
-      <c r="Y35" s="1"/>
+      <c r="V35" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="W35" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="X35" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="Y35" s="1" t="n">
+        <v>14</v>
+      </c>
       <c r="AC35" s="2"/>
       <c r="AD35" s="2"/>
       <c r="AE35" s="2"/>
@@ -1357,8 +2267,17 @@
       <c r="BG35" s="2"/>
       <c r="BH35" s="2"/>
       <c r="BI35" s="2"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BY35" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="BZ35" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="CA35" s="4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="H36" s="0" t="n">
         <v>4</v>
       </c>
@@ -1368,21 +2287,47 @@
       <c r="J36" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
-      <c r="N36" s="1"/>
+      <c r="K36" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="L36" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="M36" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="N36" s="1" t="n">
+        <v>18</v>
+      </c>
       <c r="O36" s="2"/>
-      <c r="P36" s="1"/>
-      <c r="Q36" s="1"/>
-      <c r="R36" s="1"/>
-      <c r="S36" s="1"/>
-      <c r="T36" s="1"/>
+      <c r="P36" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q36" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="R36" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="S36" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="T36" s="1" t="n">
+        <v>24</v>
+      </c>
       <c r="U36" s="2"/>
-      <c r="V36" s="1"/>
-      <c r="W36" s="1"/>
-      <c r="X36" s="1"/>
-      <c r="Y36" s="1"/>
+      <c r="V36" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="W36" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="X36" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="Y36" s="1" t="n">
+        <v>29</v>
+      </c>
       <c r="AC36" s="2"/>
       <c r="AD36" s="2"/>
       <c r="AE36" s="2"/>
@@ -1413,29 +2358,59 @@
       <c r="BG36" s="2"/>
       <c r="BH36" s="2"/>
       <c r="BI36" s="2"/>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BX36" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="BY36" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BZ36" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="CA36" s="1"/>
+    </row>
+    <row r="37" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="I37" s="0" t="n">
         <v>5</v>
       </c>
       <c r="J37" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
+      <c r="K37" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="L37" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="M37" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="N37" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="O37" s="1" t="n">
+        <v>34</v>
+      </c>
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
       <c r="R37" s="2"/>
       <c r="S37" s="2"/>
       <c r="T37" s="2"/>
-      <c r="U37" s="1"/>
-      <c r="V37" s="1"/>
-      <c r="W37" s="1"/>
-      <c r="X37" s="1"/>
-      <c r="Y37" s="1"/>
+      <c r="U37" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="V37" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="W37" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="X37" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="Y37" s="1" t="n">
+        <v>44</v>
+      </c>
       <c r="AC37" s="2"/>
       <c r="AD37" s="2"/>
       <c r="AE37" s="2"/>
@@ -1466,18 +2441,34 @@
       <c r="BG37" s="2"/>
       <c r="BH37" s="2"/>
       <c r="BI37" s="2"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BX37" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BY37" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BZ37" s="1"/>
+      <c r="CA37" s="1"/>
+    </row>
+    <row r="38" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="I38" s="0" t="n">
         <v>4</v>
       </c>
       <c r="J38" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-      <c r="N38" s="1"/>
+      <c r="K38" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="L38" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="M38" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="N38" s="1" t="n">
+        <v>48</v>
+      </c>
       <c r="O38" s="2"/>
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
@@ -1485,10 +2476,18 @@
       <c r="S38" s="2"/>
       <c r="T38" s="2"/>
       <c r="U38" s="2"/>
-      <c r="V38" s="1"/>
-      <c r="W38" s="1"/>
-      <c r="X38" s="1"/>
-      <c r="Y38" s="1"/>
+      <c r="V38" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="W38" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="X38" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="Y38" s="1" t="n">
+        <v>59</v>
+      </c>
       <c r="AC38" s="2"/>
       <c r="AD38" s="2"/>
       <c r="AE38" s="1"/>
@@ -1519,16 +2518,26 @@
       <c r="BG38" s="1"/>
       <c r="BH38" s="2"/>
       <c r="BI38" s="2"/>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BX38" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="BY38" s="1"/>
+      <c r="BZ38" s="1"/>
+      <c r="CA38" s="1"/>
+    </row>
+    <row r="39" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="I39" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J39" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
+      <c r="K39" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="L39" s="1" t="n">
+        <v>61</v>
+      </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -1540,8 +2549,12 @@
       <c r="U39" s="2"/>
       <c r="V39" s="2"/>
       <c r="W39" s="2"/>
-      <c r="X39" s="1"/>
-      <c r="Y39" s="1"/>
+      <c r="X39" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="Y39" s="1" t="n">
+        <v>74</v>
+      </c>
       <c r="AC39" s="2"/>
       <c r="AD39" s="1"/>
       <c r="AE39" s="2"/>
@@ -1573,14 +2586,16 @@
       <c r="BH39" s="2"/>
       <c r="BI39" s="2"/>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="I40" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J40" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K40" s="1"/>
+      <c r="K40" s="1" t="n">
+        <v>75</v>
+      </c>
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -1594,7 +2609,9 @@
       <c r="V40" s="2"/>
       <c r="W40" s="2"/>
       <c r="X40" s="2"/>
-      <c r="Y40" s="1"/>
+      <c r="Y40" s="1" t="n">
+        <v>89</v>
+      </c>
       <c r="AC40" s="1"/>
       <c r="AD40" s="1"/>
       <c r="AE40" s="2"/>
@@ -1626,7 +2643,7 @@
       <c r="BH40" s="1"/>
       <c r="BI40" s="2"/>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G41" s="0" t="n">
         <v>1</v>
       </c>
@@ -1639,21 +2656,37 @@
       <c r="J41" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K41" s="1"/>
+      <c r="K41" s="1" t="n">
+        <v>90</v>
+      </c>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
-      <c r="N41" s="1"/>
-      <c r="O41" s="1"/>
-      <c r="P41" s="1"/>
+      <c r="N41" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="O41" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="P41" s="1" t="n">
+        <v>95</v>
+      </c>
       <c r="Q41" s="2"/>
       <c r="R41" s="2"/>
       <c r="S41" s="2"/>
-      <c r="T41" s="1"/>
-      <c r="U41" s="1"/>
-      <c r="V41" s="1"/>
+      <c r="T41" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="U41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="V41" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="W41" s="2"/>
       <c r="X41" s="2"/>
-      <c r="Y41" s="1"/>
+      <c r="Y41" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="AC41" s="1"/>
       <c r="AD41" s="1"/>
       <c r="AE41" s="2"/>
@@ -1685,7 +2718,7 @@
       <c r="BH41" s="1"/>
       <c r="BI41" s="1"/>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G42" s="0" t="n">
         <v>4</v>
       </c>
@@ -1698,21 +2731,41 @@
       <c r="J42" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
+      <c r="K42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="O42" s="2"/>
-      <c r="P42" s="1"/>
+      <c r="P42" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="Q42" s="2"/>
       <c r="R42" s="2"/>
       <c r="S42" s="2"/>
-      <c r="T42" s="1"/>
+      <c r="T42" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="U42" s="2"/>
-      <c r="V42" s="1"/>
-      <c r="W42" s="1"/>
-      <c r="X42" s="1"/>
-      <c r="Y42" s="1"/>
+      <c r="V42" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="W42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="X42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y42" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="AC42" s="2"/>
       <c r="AD42" s="1"/>
       <c r="AE42" s="2"/>
@@ -1744,28 +2797,52 @@
       <c r="BH42" s="2"/>
       <c r="BI42" s="1"/>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="I43" s="0" t="n">
         <v>6</v>
       </c>
       <c r="J43" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="K43" s="1"/>
-      <c r="L43" s="1"/>
-      <c r="M43" s="1"/>
-      <c r="N43" s="1"/>
-      <c r="O43" s="1"/>
-      <c r="P43" s="1"/>
+      <c r="K43" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="O43" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P43" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="Q43" s="2"/>
       <c r="R43" s="2"/>
       <c r="S43" s="2"/>
-      <c r="T43" s="1"/>
-      <c r="U43" s="1"/>
-      <c r="V43" s="1"/>
-      <c r="W43" s="1"/>
-      <c r="X43" s="1"/>
-      <c r="Y43" s="1"/>
+      <c r="T43" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="U43" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="V43" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="W43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="X43" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y43" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="AC43" s="2"/>
       <c r="AD43" s="1"/>
       <c r="AE43" s="2"/>
@@ -1797,28 +2874,48 @@
       <c r="BH43" s="2"/>
       <c r="BI43" s="1"/>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="I44" s="0" t="n">
         <v>5</v>
       </c>
       <c r="J44" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
-      <c r="N44" s="1"/>
-      <c r="O44" s="1"/>
+      <c r="K44" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O44" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
       <c r="R44" s="2"/>
       <c r="S44" s="2"/>
       <c r="T44" s="2"/>
-      <c r="U44" s="1"/>
-      <c r="V44" s="1"/>
-      <c r="W44" s="1"/>
-      <c r="X44" s="1"/>
-      <c r="Y44" s="1"/>
+      <c r="U44" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="V44" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="W44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="X44" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y44" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="AC44" s="2"/>
       <c r="AD44" s="2"/>
       <c r="AE44" s="1"/>
@@ -1850,14 +2947,16 @@
       <c r="BH44" s="2"/>
       <c r="BI44" s="1"/>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="I45" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J45" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K45" s="1"/>
+      <c r="K45" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -1871,7 +2970,9 @@
       <c r="V45" s="2"/>
       <c r="W45" s="2"/>
       <c r="X45" s="2"/>
-      <c r="Y45" s="1"/>
+      <c r="Y45" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="AC45" s="2"/>
       <c r="AD45" s="2"/>
       <c r="AE45" s="2"/>
@@ -1903,7 +3004,7 @@
       <c r="BH45" s="1"/>
       <c r="BI45" s="1"/>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="H46" s="0" t="n">
         <v>1</v>
       </c>
@@ -1913,21 +3014,31 @@
       <c r="J46" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K46" s="1"/>
+      <c r="K46" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
-      <c r="Q46" s="1"/>
-      <c r="R46" s="1"/>
-      <c r="S46" s="1"/>
+      <c r="Q46" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R46" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="S46" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="T46" s="2"/>
       <c r="U46" s="2"/>
       <c r="V46" s="2"/>
       <c r="W46" s="2"/>
       <c r="X46" s="2"/>
-      <c r="Y46" s="1"/>
+      <c r="Y46" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="AC46" s="2"/>
       <c r="AD46" s="2"/>
       <c r="AE46" s="2"/>
@@ -1959,28 +3070,38 @@
       <c r="BH46" s="1"/>
       <c r="BI46" s="2"/>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="I47" s="0" t="n">
         <v>2</v>
       </c>
       <c r="J47" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="K47" s="1"/>
-      <c r="L47" s="1"/>
+      <c r="K47" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
-      <c r="R47" s="1"/>
+      <c r="R47" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="S47" s="2"/>
       <c r="T47" s="2"/>
       <c r="U47" s="2"/>
       <c r="V47" s="2"/>
       <c r="W47" s="2"/>
-      <c r="X47" s="1"/>
-      <c r="Y47" s="1"/>
+      <c r="X47" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y47" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="AC47" s="2"/>
       <c r="AD47" s="2"/>
       <c r="AE47" s="2"/>
@@ -2012,7 +3133,7 @@
       <c r="BH47" s="1"/>
       <c r="BI47" s="2"/>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G48" s="0" t="n">
         <v>1</v>
       </c>
@@ -2026,19 +3147,27 @@
         <v>1</v>
       </c>
       <c r="K48" s="2"/>
-      <c r="L48" s="1"/>
+      <c r="L48" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
       <c r="P48" s="2"/>
-      <c r="Q48" s="1"/>
+      <c r="Q48" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="R48" s="2"/>
-      <c r="S48" s="1"/>
+      <c r="S48" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="T48" s="2"/>
       <c r="U48" s="2"/>
       <c r="V48" s="2"/>
       <c r="W48" s="2"/>
-      <c r="X48" s="1"/>
+      <c r="X48" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="Y48" s="2"/>
       <c r="AC48" s="2"/>
       <c r="AD48" s="2"/>
@@ -2071,23 +3200,45 @@
       <c r="BH48" s="2"/>
       <c r="BI48" s="2"/>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="J49" s="0" t="n">
         <v>11</v>
       </c>
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
-      <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
-      <c r="O49" s="1"/>
-      <c r="P49" s="1"/>
-      <c r="Q49" s="1"/>
-      <c r="R49" s="1"/>
-      <c r="S49" s="1"/>
-      <c r="T49" s="1"/>
-      <c r="U49" s="1"/>
-      <c r="V49" s="1"/>
-      <c r="W49" s="1"/>
+      <c r="M49" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N49" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O49" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P49" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q49" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R49" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="T49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="U49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="V49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="W49" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="X49" s="2"/>
       <c r="Y49" s="2"/>
       <c r="AC49" s="2"/>
@@ -2121,17 +3272,47 @@
       <c r="BH49" s="2"/>
       <c r="BI49" s="2"/>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="R50" s="0" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="BG51" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="BH51" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BI51" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="BJ51" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="BK51" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL51" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="BM51" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="BN51" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="BO51" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="BP51" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="U52" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="V52" s="0" t="n">
         <v>2</v>
       </c>
@@ -2141,6 +3322,9 @@
       <c r="X52" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="Y52" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="AS52" s="0" t="n">
         <v>3</v>
       </c>
@@ -2171,11 +3355,23 @@
       <c r="BK52" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="BL52" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="BM52" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="BN52" s="0" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BO52" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="BP52" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="U53" s="0" t="n">
         <v>5</v>
       </c>
@@ -2267,12 +3463,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
       <c r="O54" s="2"/>
+      <c r="S54" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="T54" s="0" t="n">
         <v>5</v>
       </c>
@@ -2286,7 +3485,9 @@
       </c>
       <c r="AF54" s="2"/>
       <c r="AG54" s="2"/>
-      <c r="AH54" s="1"/>
+      <c r="AH54" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="AI54" s="2"/>
       <c r="AJ54" s="2"/>
       <c r="AN54" s="0" t="n">
@@ -2297,14 +3498,25 @@
       </c>
       <c r="AP54" s="2"/>
       <c r="AQ54" s="2"/>
-      <c r="AR54" s="1"/>
-      <c r="AS54" s="1"/>
+      <c r="AR54" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="AS54" s="1" t="n">
+        <v>3</v>
+      </c>
       <c r="AT54" s="2"/>
       <c r="AU54" s="2"/>
-      <c r="AV54" s="1"/>
-      <c r="AW54" s="1"/>
+      <c r="AV54" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="AW54" s="1" t="n">
+        <v>7</v>
+      </c>
       <c r="AX54" s="2"/>
       <c r="AY54" s="2"/>
+      <c r="BD54" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="BE54" s="0" t="n">
         <v>1</v>
       </c>
@@ -2312,9 +3524,13 @@
         <v>1</v>
       </c>
       <c r="BG54" s="2"/>
-      <c r="BH54" s="1"/>
+      <c r="BH54" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="BI54" s="2"/>
-      <c r="BJ54" s="1"/>
+      <c r="BJ54" s="1" t="n">
+        <v>3</v>
+      </c>
       <c r="BK54" s="2"/>
       <c r="BL54" s="2"/>
       <c r="BM54" s="2"/>
@@ -2322,7 +3538,7 @@
       <c r="BO54" s="2"/>
       <c r="BP54" s="2"/>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
@@ -2344,21 +3560,41 @@
       </c>
       <c r="AF55" s="2"/>
       <c r="AG55" s="2"/>
-      <c r="AH55" s="1"/>
-      <c r="AI55" s="1"/>
+      <c r="AH55" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="AI55" s="1" t="n">
+        <v>8</v>
+      </c>
       <c r="AJ55" s="2"/>
       <c r="AO55" s="0" t="n">
         <v>8</v>
       </c>
       <c r="AP55" s="2"/>
-      <c r="AQ55" s="1"/>
-      <c r="AR55" s="1"/>
-      <c r="AS55" s="1"/>
-      <c r="AT55" s="1"/>
-      <c r="AU55" s="1"/>
-      <c r="AV55" s="1"/>
-      <c r="AW55" s="1"/>
-      <c r="AX55" s="1"/>
+      <c r="AQ55" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="AR55" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="AS55" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="AT55" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="AU55" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="AV55" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="AW55" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="AX55" s="1" t="n">
+        <v>18</v>
+      </c>
       <c r="AY55" s="2"/>
       <c r="BD55" s="0" t="n">
         <v>1</v>
@@ -2369,18 +3605,24 @@
       <c r="BF55" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="BG55" s="1"/>
+      <c r="BG55" s="1" t="n">
+        <v>10</v>
+      </c>
       <c r="BH55" s="2"/>
-      <c r="BI55" s="1"/>
+      <c r="BI55" s="1" t="n">
+        <v>12</v>
+      </c>
       <c r="BJ55" s="2"/>
-      <c r="BK55" s="1"/>
+      <c r="BK55" s="1" t="n">
+        <v>14</v>
+      </c>
       <c r="BL55" s="2"/>
       <c r="BM55" s="2"/>
       <c r="BN55" s="2"/>
       <c r="BO55" s="2"/>
       <c r="BP55" s="2"/>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
       <c r="M56" s="2"/>
@@ -2405,9 +3647,13 @@
       </c>
       <c r="AF56" s="2"/>
       <c r="AG56" s="2"/>
-      <c r="AH56" s="1"/>
+      <c r="AH56" s="1" t="n">
+        <v>12</v>
+      </c>
       <c r="AI56" s="2"/>
-      <c r="AJ56" s="1"/>
+      <c r="AJ56" s="1" t="n">
+        <v>14</v>
+      </c>
       <c r="AM56" s="0" t="n">
         <v>4</v>
       </c>
@@ -2417,22 +3663,46 @@
       <c r="AO56" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="AP56" s="1"/>
-      <c r="AQ56" s="1"/>
-      <c r="AR56" s="1"/>
-      <c r="AS56" s="1"/>
+      <c r="AP56" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ56" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="AR56" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="AS56" s="1" t="n">
+        <v>23</v>
+      </c>
       <c r="AT56" s="2"/>
-      <c r="AU56" s="1"/>
+      <c r="AU56" s="1" t="n">
+        <v>25</v>
+      </c>
       <c r="AV56" s="2"/>
-      <c r="AW56" s="1"/>
-      <c r="AX56" s="1"/>
-      <c r="AY56" s="1"/>
+      <c r="AW56" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="AX56" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="AY56" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="BD56" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="BE56" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="BF56" s="0" t="n">
         <v>1</v>
       </c>
       <c r="BG56" s="2"/>
       <c r="BH56" s="2"/>
-      <c r="BI56" s="1"/>
+      <c r="BI56" s="1" t="n">
+        <v>22</v>
+      </c>
       <c r="BJ56" s="2"/>
       <c r="BK56" s="2"/>
       <c r="BL56" s="2"/>
@@ -2441,7 +3711,7 @@
       <c r="BO56" s="2"/>
       <c r="BP56" s="2"/>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
       <c r="M57" s="2"/>
@@ -2461,9 +3731,15 @@
       <c r="AE57" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="AF57" s="1"/>
-      <c r="AG57" s="1"/>
-      <c r="AH57" s="1"/>
+      <c r="AF57" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="AG57" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="AH57" s="1" t="n">
+        <v>17</v>
+      </c>
       <c r="AI57" s="2"/>
       <c r="AJ57" s="2"/>
       <c r="AN57" s="0" t="n">
@@ -2472,16 +3748,32 @@
       <c r="AO57" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="AP57" s="1"/>
-      <c r="AQ57" s="1"/>
-      <c r="AR57" s="1"/>
+      <c r="AP57" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="AQ57" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="AR57" s="1" t="n">
+        <v>32</v>
+      </c>
       <c r="AS57" s="2"/>
       <c r="AT57" s="2"/>
       <c r="AU57" s="2"/>
       <c r="AV57" s="2"/>
       <c r="AW57" s="2"/>
-      <c r="AX57" s="1"/>
-      <c r="AY57" s="1"/>
+      <c r="AX57" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="AY57" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="BD57" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="BE57" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="BF57" s="0" t="n">
         <v>0</v>
       </c>
@@ -2496,12 +3788,15 @@
       <c r="BO57" s="2"/>
       <c r="BP57" s="2"/>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
       <c r="O58" s="2"/>
+      <c r="S58" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="T58" s="0" t="n">
         <v>5</v>
       </c>
@@ -2513,9 +3808,15 @@
       <c r="AE58" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="AF58" s="1"/>
-      <c r="AG58" s="1"/>
-      <c r="AH58" s="1"/>
+      <c r="AF58" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG58" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="AH58" s="1" t="n">
+        <v>22</v>
+      </c>
       <c r="AI58" s="2"/>
       <c r="AJ58" s="2"/>
       <c r="AN58" s="0" t="n">
@@ -2524,16 +3825,26 @@
       <c r="AO58" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="AP58" s="1"/>
-      <c r="AQ58" s="1"/>
-      <c r="AR58" s="1"/>
+      <c r="AP58" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="AQ58" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="AR58" s="1" t="n">
+        <v>42</v>
+      </c>
       <c r="AS58" s="2"/>
       <c r="AT58" s="2"/>
       <c r="AU58" s="2"/>
       <c r="AV58" s="2"/>
       <c r="AW58" s="2"/>
-      <c r="AX58" s="1"/>
-      <c r="AY58" s="1"/>
+      <c r="AX58" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="AY58" s="1" t="n">
+        <v>49</v>
+      </c>
       <c r="BD58" s="0" t="n">
         <v>4</v>
       </c>
@@ -2544,22 +3855,34 @@
         <v>1</v>
       </c>
       <c r="BG58" s="2"/>
-      <c r="BH58" s="1"/>
-      <c r="BI58" s="1"/>
-      <c r="BJ58" s="1"/>
-      <c r="BK58" s="1"/>
+      <c r="BH58" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="BI58" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="BJ58" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="BK58" s="1" t="n">
+        <v>44</v>
+      </c>
       <c r="BL58" s="2"/>
       <c r="BM58" s="2"/>
-      <c r="BN58" s="1"/>
+      <c r="BN58" s="1" t="n">
+        <v>47</v>
+      </c>
       <c r="BO58" s="2"/>
-      <c r="BP58" s="1"/>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP58" s="1" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="W59" s="0" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="AH59" s="0" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="AN59" s="0" t="n">
         <v>4</v>
@@ -2567,34 +3890,69 @@
       <c r="AO59" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="AP59" s="1"/>
-      <c r="AQ59" s="1"/>
-      <c r="AR59" s="1"/>
-      <c r="AS59" s="1"/>
+      <c r="AP59" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="AQ59" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="AR59" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="AS59" s="1" t="n">
+        <v>53</v>
+      </c>
       <c r="AT59" s="2"/>
       <c r="AU59" s="2"/>
       <c r="AV59" s="2"/>
-      <c r="AW59" s="1"/>
-      <c r="AX59" s="1"/>
-      <c r="AY59" s="1"/>
+      <c r="AW59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="AX59" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="AY59" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="BD59" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="BE59" s="0" t="n">
         <v>6</v>
       </c>
       <c r="BF59" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="BG59" s="1"/>
-      <c r="BH59" s="1"/>
-      <c r="BI59" s="1"/>
-      <c r="BJ59" s="1"/>
-      <c r="BK59" s="1"/>
-      <c r="BL59" s="1"/>
+      <c r="BG59" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="BH59" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="BI59" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="BJ59" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="BK59" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="BL59" s="1" t="n">
+        <v>55</v>
+      </c>
       <c r="BM59" s="2"/>
-      <c r="BN59" s="1"/>
-      <c r="BO59" s="1"/>
-      <c r="BP59" s="1"/>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BN59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="BO59" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="BP59" s="1" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="AN60" s="0" t="n">
         <v>4</v>
       </c>
@@ -2602,14 +3960,28 @@
         <v>3</v>
       </c>
       <c r="AP60" s="2"/>
-      <c r="AQ60" s="1"/>
-      <c r="AR60" s="1"/>
-      <c r="AS60" s="1"/>
-      <c r="AT60" s="1"/>
+      <c r="AQ60" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="AR60" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="AS60" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="AT60" s="1" t="n">
+        <v>64</v>
+      </c>
       <c r="AU60" s="2"/>
-      <c r="AV60" s="1"/>
-      <c r="AW60" s="1"/>
-      <c r="AX60" s="1"/>
+      <c r="AV60" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="AW60" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="AX60" s="1" t="n">
+        <v>68</v>
+      </c>
       <c r="AY60" s="2"/>
       <c r="BD60" s="0" t="n">
         <v>1</v>
@@ -2620,74 +3992,253 @@
       <c r="BF60" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="BG60" s="1"/>
+      <c r="BG60" s="1" t="n">
+        <v>60</v>
+      </c>
       <c r="BH60" s="2"/>
-      <c r="BI60" s="1"/>
-      <c r="BJ60" s="1"/>
-      <c r="BK60" s="1"/>
-      <c r="BL60" s="1"/>
-      <c r="BM60" s="1"/>
+      <c r="BI60" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="BJ60" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="BK60" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="BL60" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="BM60" s="1" t="n">
+        <v>66</v>
+      </c>
       <c r="BN60" s="2"/>
-      <c r="BO60" s="1"/>
-      <c r="BP60" s="1"/>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BO60" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="BP60" s="1" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="S61" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="T61" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="U61" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="V61" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="W61" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="X61" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y61" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z61" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA61" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="AF61" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG61" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="AH61" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AI61" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="AJ61" s="0" t="n">
+        <v>14</v>
+      </c>
       <c r="AO61" s="0" t="n">
         <v>6</v>
       </c>
       <c r="AP61" s="2"/>
       <c r="AQ61" s="2"/>
-      <c r="AR61" s="1"/>
-      <c r="AS61" s="1"/>
-      <c r="AT61" s="1"/>
-      <c r="AU61" s="1"/>
-      <c r="AV61" s="1"/>
-      <c r="AW61" s="1"/>
+      <c r="AR61" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="AS61" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="AT61" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="AU61" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="AV61" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="AW61" s="1" t="n">
+        <v>77</v>
+      </c>
       <c r="AX61" s="2"/>
       <c r="AY61" s="2"/>
+      <c r="BD61" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="BE61" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="BF61" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="BG61" s="1"/>
-      <c r="BH61" s="1"/>
-      <c r="BI61" s="1"/>
-      <c r="BJ61" s="1"/>
-      <c r="BK61" s="1"/>
-      <c r="BL61" s="1"/>
-      <c r="BM61" s="1"/>
-      <c r="BN61" s="1"/>
-      <c r="BO61" s="1"/>
-      <c r="BP61" s="1"/>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BG61" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="BH61" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="BI61" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="BJ61" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="BK61" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="BL61" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="BM61" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="BN61" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="BO61" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="BP61" s="1" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="S62" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="T62" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="U62" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="V62" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="W62" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="X62" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="Y62" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="Z62" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AA62" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="AF62" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="AG62" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="AH62" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="AI62" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="AJ62" s="0" t="n">
+        <v>21</v>
+      </c>
       <c r="AO62" s="0" t="n">
         <v>4</v>
       </c>
       <c r="AP62" s="2"/>
       <c r="AQ62" s="2"/>
       <c r="AR62" s="2"/>
-      <c r="AS62" s="1"/>
-      <c r="AT62" s="1"/>
-      <c r="AU62" s="1"/>
-      <c r="AV62" s="1"/>
+      <c r="AS62" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="AT62" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="AU62" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="AV62" s="1" t="n">
+        <v>86</v>
+      </c>
       <c r="AW62" s="2"/>
       <c r="AX62" s="2"/>
       <c r="AY62" s="2"/>
+      <c r="BD62" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="BE62" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="BF62" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="BG62" s="1"/>
-      <c r="BH62" s="1"/>
-      <c r="BI62" s="1"/>
-      <c r="BJ62" s="1"/>
-      <c r="BK62" s="1"/>
-      <c r="BL62" s="1"/>
-      <c r="BM62" s="1"/>
-      <c r="BN62" s="1"/>
-      <c r="BO62" s="1"/>
+      <c r="BG62" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="BH62" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="BI62" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="BJ62" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="BK62" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="BL62" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="BM62" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="BN62" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="BO62" s="1" t="n">
+        <v>88</v>
+      </c>
       <c r="BP62" s="2"/>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="S63" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="T63" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="AF63" s="0" t="n">
+        <v>22</v>
+      </c>
       <c r="AO63" s="0" t="n">
         <v>2</v>
       </c>
@@ -2695,35 +4246,70 @@
       <c r="AQ63" s="2"/>
       <c r="AR63" s="2"/>
       <c r="AS63" s="2"/>
-      <c r="AT63" s="1"/>
-      <c r="AU63" s="1"/>
+      <c r="AT63" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="AU63" s="1" t="n">
+        <v>95</v>
+      </c>
       <c r="AV63" s="2"/>
       <c r="AW63" s="2"/>
       <c r="AX63" s="2"/>
       <c r="AY63" s="2"/>
+      <c r="BD63" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="BE63" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="BF63" s="0" t="n">
         <v>7</v>
       </c>
       <c r="BG63" s="2"/>
-      <c r="BH63" s="1"/>
-      <c r="BI63" s="1"/>
-      <c r="BJ63" s="1"/>
-      <c r="BK63" s="1"/>
-      <c r="BL63" s="1"/>
-      <c r="BM63" s="1"/>
-      <c r="BN63" s="1"/>
+      <c r="BH63" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="BI63" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="BJ63" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="BK63" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="BL63" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="BM63" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="BN63" s="1" t="n">
+        <v>97</v>
+      </c>
       <c r="BO63" s="2"/>
       <c r="BP63" s="2"/>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="H64" s="0" t="s">
-        <v>1</v>
+        <v>81</v>
       </c>
       <c r="AT64" s="0" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="BK64" s="0" t="s">
-        <v>0</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="X68" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="Y68" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="Z68" s="0" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added timer feature, ability to use keyboard for controls, and rating for game completion
</commit_message>
<xml_diff>
--- a/assets/Logic Square References.xlsx
+++ b/assets/Logic Square References.xlsx
@@ -359,16 +359,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -459,8 +455,8 @@
   </sheetPr>
   <dimension ref="G5:CE68"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S63" activeCellId="0" sqref="I43:S63"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.3" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -736,21 +732,21 @@
       <c r="BG9" s="2"/>
       <c r="BH9" s="2"/>
       <c r="BI9" s="2"/>
-      <c r="BQ9" s="3"/>
-      <c r="BR9" s="3"/>
-      <c r="BS9" s="3"/>
-      <c r="BT9" s="3"/>
-      <c r="BU9" s="3"/>
-      <c r="BV9" s="3"/>
-      <c r="BW9" s="3"/>
-      <c r="BX9" s="3"/>
-      <c r="BY9" s="3"/>
-      <c r="BZ9" s="3"/>
-      <c r="CA9" s="3"/>
-      <c r="CB9" s="3"/>
-      <c r="CC9" s="3"/>
-      <c r="CD9" s="3"/>
-      <c r="CE9" s="3"/>
+      <c r="BQ9" s="2"/>
+      <c r="BR9" s="2"/>
+      <c r="BS9" s="2"/>
+      <c r="BT9" s="2"/>
+      <c r="BU9" s="2"/>
+      <c r="BV9" s="2"/>
+      <c r="BW9" s="2"/>
+      <c r="BX9" s="2"/>
+      <c r="BY9" s="2"/>
+      <c r="BZ9" s="2"/>
+      <c r="CA9" s="2"/>
+      <c r="CB9" s="2"/>
+      <c r="CC9" s="2"/>
+      <c r="CD9" s="2"/>
+      <c r="CE9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G10" s="0" t="s">
@@ -840,21 +836,21 @@
       <c r="BG10" s="1"/>
       <c r="BH10" s="1"/>
       <c r="BI10" s="1"/>
-      <c r="BQ10" s="3"/>
-      <c r="BR10" s="3"/>
-      <c r="BS10" s="3"/>
-      <c r="BT10" s="3"/>
-      <c r="BU10" s="3"/>
-      <c r="BV10" s="3"/>
+      <c r="BQ10" s="2"/>
+      <c r="BR10" s="2"/>
+      <c r="BS10" s="2"/>
+      <c r="BT10" s="2"/>
+      <c r="BU10" s="2"/>
+      <c r="BV10" s="2"/>
       <c r="BW10" s="1"/>
       <c r="BX10" s="1"/>
       <c r="BY10" s="1"/>
-      <c r="BZ10" s="3"/>
-      <c r="CA10" s="3"/>
-      <c r="CB10" s="3"/>
-      <c r="CC10" s="3"/>
-      <c r="CD10" s="3"/>
-      <c r="CE10" s="3"/>
+      <c r="BZ10" s="2"/>
+      <c r="CA10" s="2"/>
+      <c r="CB10" s="2"/>
+      <c r="CC10" s="2"/>
+      <c r="CD10" s="2"/>
+      <c r="CE10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G11" s="0" t="s">
@@ -944,21 +940,21 @@
       <c r="BG11" s="2"/>
       <c r="BH11" s="2"/>
       <c r="BI11" s="1"/>
-      <c r="BQ11" s="3"/>
-      <c r="BR11" s="3"/>
-      <c r="BS11" s="3"/>
-      <c r="BT11" s="3"/>
+      <c r="BQ11" s="2"/>
+      <c r="BR11" s="2"/>
+      <c r="BS11" s="2"/>
+      <c r="BT11" s="2"/>
       <c r="BU11" s="1"/>
       <c r="BV11" s="1"/>
       <c r="BW11" s="1"/>
       <c r="BX11" s="1"/>
       <c r="BY11" s="1"/>
       <c r="BZ11" s="1"/>
-      <c r="CA11" s="3"/>
-      <c r="CB11" s="3"/>
-      <c r="CC11" s="3"/>
-      <c r="CD11" s="3"/>
-      <c r="CE11" s="3"/>
+      <c r="CA11" s="2"/>
+      <c r="CB11" s="2"/>
+      <c r="CC11" s="2"/>
+      <c r="CD11" s="2"/>
+      <c r="CE11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G12" s="0" t="s">
@@ -1040,21 +1036,21 @@
       <c r="BG12" s="2"/>
       <c r="BH12" s="1"/>
       <c r="BI12" s="2"/>
-      <c r="BQ12" s="3"/>
-      <c r="BR12" s="3"/>
-      <c r="BS12" s="3"/>
+      <c r="BQ12" s="2"/>
+      <c r="BR12" s="2"/>
+      <c r="BS12" s="2"/>
       <c r="BT12" s="1"/>
       <c r="BU12" s="1"/>
       <c r="BV12" s="1"/>
-      <c r="BW12" s="3"/>
-      <c r="BX12" s="3"/>
-      <c r="BY12" s="3"/>
+      <c r="BW12" s="2"/>
+      <c r="BX12" s="2"/>
+      <c r="BY12" s="2"/>
       <c r="BZ12" s="1"/>
       <c r="CA12" s="1"/>
-      <c r="CB12" s="3"/>
-      <c r="CC12" s="3"/>
-      <c r="CD12" s="3"/>
-      <c r="CE12" s="3"/>
+      <c r="CB12" s="2"/>
+      <c r="CC12" s="2"/>
+      <c r="CD12" s="2"/>
+      <c r="CE12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G13" s="0" t="s">
@@ -1118,21 +1114,21 @@
       <c r="BG13" s="1"/>
       <c r="BH13" s="2"/>
       <c r="BI13" s="2"/>
-      <c r="BQ13" s="3"/>
-      <c r="BR13" s="3"/>
-      <c r="BS13" s="3"/>
+      <c r="BQ13" s="2"/>
+      <c r="BR13" s="2"/>
+      <c r="BS13" s="2"/>
       <c r="BT13" s="1"/>
       <c r="BU13" s="1"/>
-      <c r="BV13" s="3"/>
-      <c r="BW13" s="3"/>
-      <c r="BX13" s="3"/>
-      <c r="BY13" s="3"/>
-      <c r="BZ13" s="3"/>
+      <c r="BV13" s="2"/>
+      <c r="BW13" s="2"/>
+      <c r="BX13" s="2"/>
+      <c r="BY13" s="2"/>
+      <c r="BZ13" s="2"/>
       <c r="CA13" s="1"/>
       <c r="CB13" s="1"/>
-      <c r="CC13" s="3"/>
-      <c r="CD13" s="3"/>
-      <c r="CE13" s="3"/>
+      <c r="CC13" s="2"/>
+      <c r="CD13" s="2"/>
+      <c r="CE13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G14" s="0" t="s">
@@ -1200,21 +1196,21 @@
       <c r="BG14" s="2"/>
       <c r="BH14" s="2"/>
       <c r="BI14" s="2"/>
-      <c r="BQ14" s="3"/>
-      <c r="BR14" s="3"/>
-      <c r="BS14" s="3"/>
-      <c r="BT14" s="3"/>
-      <c r="BU14" s="3"/>
-      <c r="BV14" s="3"/>
-      <c r="BW14" s="3"/>
-      <c r="BX14" s="3"/>
-      <c r="BY14" s="3"/>
-      <c r="BZ14" s="3"/>
+      <c r="BQ14" s="2"/>
+      <c r="BR14" s="2"/>
+      <c r="BS14" s="2"/>
+      <c r="BT14" s="2"/>
+      <c r="BU14" s="2"/>
+      <c r="BV14" s="2"/>
+      <c r="BW14" s="2"/>
+      <c r="BX14" s="2"/>
+      <c r="BY14" s="2"/>
+      <c r="BZ14" s="2"/>
       <c r="CA14" s="1"/>
       <c r="CB14" s="1"/>
-      <c r="CC14" s="3"/>
-      <c r="CD14" s="3"/>
-      <c r="CE14" s="3"/>
+      <c r="CC14" s="2"/>
+      <c r="CD14" s="2"/>
+      <c r="CE14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G15" s="0" t="n">
@@ -1298,21 +1294,21 @@
       <c r="BG15" s="1"/>
       <c r="BH15" s="1"/>
       <c r="BI15" s="2"/>
-      <c r="BQ15" s="3"/>
-      <c r="BR15" s="3"/>
-      <c r="BS15" s="3"/>
-      <c r="BT15" s="3"/>
-      <c r="BU15" s="3"/>
-      <c r="BV15" s="3"/>
-      <c r="BW15" s="3"/>
-      <c r="BX15" s="3"/>
-      <c r="BY15" s="3"/>
-      <c r="BZ15" s="3"/>
+      <c r="BQ15" s="2"/>
+      <c r="BR15" s="2"/>
+      <c r="BS15" s="2"/>
+      <c r="BT15" s="2"/>
+      <c r="BU15" s="2"/>
+      <c r="BV15" s="2"/>
+      <c r="BW15" s="2"/>
+      <c r="BX15" s="2"/>
+      <c r="BY15" s="2"/>
+      <c r="BZ15" s="2"/>
       <c r="CA15" s="1"/>
       <c r="CB15" s="1"/>
-      <c r="CC15" s="3"/>
-      <c r="CD15" s="3"/>
-      <c r="CE15" s="3"/>
+      <c r="CC15" s="2"/>
+      <c r="CD15" s="2"/>
+      <c r="CE15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G16" s="0" t="n">
@@ -1388,21 +1384,21 @@
       <c r="BG16" s="2"/>
       <c r="BH16" s="1"/>
       <c r="BI16" s="2"/>
-      <c r="BQ16" s="3"/>
-      <c r="BR16" s="3"/>
-      <c r="BS16" s="3"/>
-      <c r="BT16" s="3"/>
-      <c r="BU16" s="3"/>
-      <c r="BV16" s="3"/>
+      <c r="BQ16" s="2"/>
+      <c r="BR16" s="2"/>
+      <c r="BS16" s="2"/>
+      <c r="BT16" s="2"/>
+      <c r="BU16" s="2"/>
+      <c r="BV16" s="2"/>
       <c r="BW16" s="1"/>
       <c r="BX16" s="1"/>
       <c r="BY16" s="1"/>
       <c r="BZ16" s="1"/>
       <c r="CA16" s="1"/>
-      <c r="CB16" s="3"/>
-      <c r="CC16" s="3"/>
-      <c r="CD16" s="3"/>
-      <c r="CE16" s="3"/>
+      <c r="CB16" s="2"/>
+      <c r="CC16" s="2"/>
+      <c r="CD16" s="2"/>
+      <c r="CE16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G17" s="0" t="s">
@@ -1474,31 +1470,28 @@
       <c r="BG17" s="1"/>
       <c r="BH17" s="2"/>
       <c r="BI17" s="2"/>
-      <c r="BQ17" s="3"/>
-      <c r="BR17" s="3"/>
-      <c r="BS17" s="3"/>
-      <c r="BT17" s="3"/>
-      <c r="BU17" s="3"/>
+      <c r="BQ17" s="2"/>
+      <c r="BR17" s="2"/>
+      <c r="BS17" s="2"/>
+      <c r="BT17" s="2"/>
+      <c r="BU17" s="2"/>
       <c r="BV17" s="1"/>
       <c r="BW17" s="1"/>
       <c r="BX17" s="1"/>
       <c r="BY17" s="1"/>
       <c r="BZ17" s="1"/>
       <c r="CA17" s="1"/>
-      <c r="CB17" s="3"/>
-      <c r="CC17" s="3"/>
-      <c r="CD17" s="3"/>
-      <c r="CE17" s="3"/>
+      <c r="CB17" s="2"/>
+      <c r="CC17" s="2"/>
+      <c r="CD17" s="2"/>
+      <c r="CE17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G18" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="H18" s="0" t="n">
-        <v>3</v>
-      </c>
       <c r="I18" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J18" s="0" t="n">
         <v>3</v>
@@ -1560,21 +1553,21 @@
       <c r="BG18" s="1"/>
       <c r="BH18" s="1"/>
       <c r="BI18" s="2"/>
-      <c r="BQ18" s="3"/>
-      <c r="BR18" s="3"/>
-      <c r="BS18" s="3"/>
-      <c r="BT18" s="3"/>
-      <c r="BU18" s="3"/>
+      <c r="BQ18" s="2"/>
+      <c r="BR18" s="2"/>
+      <c r="BS18" s="2"/>
+      <c r="BT18" s="2"/>
+      <c r="BU18" s="2"/>
       <c r="BV18" s="1"/>
       <c r="BW18" s="1"/>
-      <c r="BX18" s="3"/>
-      <c r="BY18" s="3"/>
-      <c r="BZ18" s="3"/>
-      <c r="CA18" s="3"/>
-      <c r="CB18" s="3"/>
-      <c r="CC18" s="3"/>
-      <c r="CD18" s="3"/>
-      <c r="CE18" s="3"/>
+      <c r="BX18" s="2"/>
+      <c r="BY18" s="2"/>
+      <c r="BZ18" s="2"/>
+      <c r="CA18" s="2"/>
+      <c r="CB18" s="2"/>
+      <c r="CC18" s="2"/>
+      <c r="CD18" s="2"/>
+      <c r="CE18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G19" s="0" t="s">
@@ -1648,21 +1641,21 @@
       <c r="BG19" s="1"/>
       <c r="BH19" s="2"/>
       <c r="BI19" s="2"/>
-      <c r="BQ19" s="3"/>
-      <c r="BR19" s="3"/>
-      <c r="BS19" s="3"/>
-      <c r="BT19" s="3"/>
-      <c r="BU19" s="3"/>
+      <c r="BQ19" s="2"/>
+      <c r="BR19" s="2"/>
+      <c r="BS19" s="2"/>
+      <c r="BT19" s="2"/>
+      <c r="BU19" s="2"/>
       <c r="BV19" s="1"/>
       <c r="BW19" s="1"/>
-      <c r="BX19" s="3"/>
-      <c r="BY19" s="3"/>
-      <c r="BZ19" s="3"/>
-      <c r="CA19" s="3"/>
-      <c r="CB19" s="3"/>
-      <c r="CC19" s="3"/>
-      <c r="CD19" s="3"/>
-      <c r="CE19" s="3"/>
+      <c r="BX19" s="2"/>
+      <c r="BY19" s="2"/>
+      <c r="BZ19" s="2"/>
+      <c r="CA19" s="2"/>
+      <c r="CB19" s="2"/>
+      <c r="CC19" s="2"/>
+      <c r="CD19" s="2"/>
+      <c r="CE19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G20" s="0" t="n">
@@ -1742,21 +1735,21 @@
       <c r="BG20" s="2"/>
       <c r="BH20" s="2"/>
       <c r="BI20" s="2"/>
-      <c r="BQ20" s="3"/>
-      <c r="BR20" s="3"/>
-      <c r="BS20" s="3"/>
-      <c r="BT20" s="3"/>
-      <c r="BU20" s="3"/>
-      <c r="BV20" s="3"/>
-      <c r="BW20" s="3"/>
-      <c r="BX20" s="3"/>
-      <c r="BY20" s="3"/>
-      <c r="BZ20" s="3"/>
-      <c r="CA20" s="3"/>
-      <c r="CB20" s="3"/>
-      <c r="CC20" s="3"/>
-      <c r="CD20" s="3"/>
-      <c r="CE20" s="3"/>
+      <c r="BQ20" s="2"/>
+      <c r="BR20" s="2"/>
+      <c r="BS20" s="2"/>
+      <c r="BT20" s="2"/>
+      <c r="BU20" s="2"/>
+      <c r="BV20" s="2"/>
+      <c r="BW20" s="2"/>
+      <c r="BX20" s="2"/>
+      <c r="BY20" s="2"/>
+      <c r="BZ20" s="2"/>
+      <c r="CA20" s="2"/>
+      <c r="CB20" s="2"/>
+      <c r="CC20" s="2"/>
+      <c r="CD20" s="2"/>
+      <c r="CE20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G21" s="0" t="s">
@@ -1836,21 +1829,21 @@
       <c r="BG21" s="2"/>
       <c r="BH21" s="2"/>
       <c r="BI21" s="2"/>
-      <c r="BQ21" s="3"/>
-      <c r="BR21" s="3"/>
-      <c r="BS21" s="3"/>
-      <c r="BT21" s="3"/>
-      <c r="BU21" s="3"/>
+      <c r="BQ21" s="2"/>
+      <c r="BR21" s="2"/>
+      <c r="BS21" s="2"/>
+      <c r="BT21" s="2"/>
+      <c r="BU21" s="2"/>
       <c r="BV21" s="1"/>
       <c r="BW21" s="1"/>
-      <c r="BX21" s="3"/>
-      <c r="BY21" s="3"/>
-      <c r="BZ21" s="3"/>
-      <c r="CA21" s="3"/>
-      <c r="CB21" s="3"/>
-      <c r="CC21" s="3"/>
-      <c r="CD21" s="3"/>
-      <c r="CE21" s="3"/>
+      <c r="BX21" s="2"/>
+      <c r="BY21" s="2"/>
+      <c r="BZ21" s="2"/>
+      <c r="CA21" s="2"/>
+      <c r="CB21" s="2"/>
+      <c r="CC21" s="2"/>
+      <c r="CD21" s="2"/>
+      <c r="CE21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G22" s="0" t="s">
@@ -1940,21 +1933,21 @@
       <c r="BG22" s="2"/>
       <c r="BH22" s="2"/>
       <c r="BI22" s="2"/>
-      <c r="BQ22" s="3"/>
-      <c r="BR22" s="3"/>
-      <c r="BS22" s="3"/>
-      <c r="BT22" s="3"/>
-      <c r="BU22" s="3"/>
+      <c r="BQ22" s="2"/>
+      <c r="BR22" s="2"/>
+      <c r="BS22" s="2"/>
+      <c r="BT22" s="2"/>
+      <c r="BU22" s="2"/>
       <c r="BV22" s="1"/>
       <c r="BW22" s="1"/>
-      <c r="BX22" s="3"/>
-      <c r="BY22" s="3"/>
-      <c r="BZ22" s="3"/>
-      <c r="CA22" s="3"/>
-      <c r="CB22" s="3"/>
-      <c r="CC22" s="3"/>
-      <c r="CD22" s="3"/>
-      <c r="CE22" s="3"/>
+      <c r="BX22" s="2"/>
+      <c r="BY22" s="2"/>
+      <c r="BZ22" s="2"/>
+      <c r="CA22" s="2"/>
+      <c r="CB22" s="2"/>
+      <c r="CC22" s="2"/>
+      <c r="CD22" s="2"/>
+      <c r="CE22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G23" s="0" t="s">
@@ -2036,21 +2029,21 @@
       <c r="BG23" s="2"/>
       <c r="BH23" s="2"/>
       <c r="BI23" s="2"/>
-      <c r="BQ23" s="3"/>
-      <c r="BR23" s="3"/>
-      <c r="BS23" s="3"/>
-      <c r="BT23" s="3"/>
-      <c r="BU23" s="3"/>
-      <c r="BV23" s="3"/>
-      <c r="BW23" s="3"/>
-      <c r="BX23" s="3"/>
-      <c r="BY23" s="3"/>
-      <c r="BZ23" s="3"/>
-      <c r="CA23" s="3"/>
-      <c r="CB23" s="3"/>
-      <c r="CC23" s="3"/>
-      <c r="CD23" s="3"/>
-      <c r="CE23" s="3"/>
+      <c r="BQ23" s="2"/>
+      <c r="BR23" s="2"/>
+      <c r="BS23" s="2"/>
+      <c r="BT23" s="2"/>
+      <c r="BU23" s="2"/>
+      <c r="BV23" s="2"/>
+      <c r="BW23" s="2"/>
+      <c r="BX23" s="2"/>
+      <c r="BY23" s="2"/>
+      <c r="BZ23" s="2"/>
+      <c r="CA23" s="2"/>
+      <c r="CB23" s="2"/>
+      <c r="CC23" s="2"/>
+      <c r="CD23" s="2"/>
+      <c r="CE23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="R24" s="0" t="s">
@@ -2267,13 +2260,13 @@
       <c r="BG35" s="2"/>
       <c r="BH35" s="2"/>
       <c r="BI35" s="2"/>
-      <c r="BY35" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BZ35" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="CA35" s="4" t="n">
+      <c r="BY35" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BZ35" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="CA35" s="3" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2358,7 +2351,7 @@
       <c r="BG36" s="2"/>
       <c r="BH36" s="2"/>
       <c r="BI36" s="2"/>
-      <c r="BX36" s="4" t="n">
+      <c r="BX36" s="3" t="n">
         <v>1</v>
       </c>
       <c r="BY36" s="2" t="s">
@@ -2441,7 +2434,7 @@
       <c r="BG37" s="2"/>
       <c r="BH37" s="2"/>
       <c r="BI37" s="2"/>
-      <c r="BX37" s="4" t="n">
+      <c r="BX37" s="3" t="n">
         <v>2</v>
       </c>
       <c r="BY37" s="2" t="s">
@@ -2518,7 +2511,7 @@
       <c r="BG38" s="1"/>
       <c r="BH38" s="2"/>
       <c r="BI38" s="2"/>
-      <c r="BX38" s="4" t="n">
+      <c r="BX38" s="3" t="n">
         <v>3</v>
       </c>
       <c r="BY38" s="1"/>

</xml_diff>